<commit_message>
professors.xls updated with valid information
</commit_message>
<xml_diff>
--- a/projeto/calendar_generator_engine/src/test/java/professors.xlsx
+++ b/projeto/calendar_generator_engine/src/test/java/professors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duarte\Documents\GitHub\examCalendar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duarte\Documents\GitHub\examCalendar\projeto\calendar_generator_engine\src\test\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,40 +24,203 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
   <si>
     <t>EIC0009</t>
   </si>
   <si>
-    <t>trigo</t>
-  </si>
-  <si>
     <t>EIC0105</t>
   </si>
   <si>
     <t>EIC0028</t>
   </si>
   <si>
-    <t>mest</t>
-  </si>
-  <si>
-    <t>einstein</t>
-  </si>
-  <si>
-    <t>rma</t>
+    <t>jtb</t>
+  </si>
+  <si>
+    <t>jev</t>
+  </si>
+  <si>
+    <t>EIC0010</t>
+  </si>
+  <si>
+    <t>jlmb</t>
+  </si>
+  <si>
+    <t>jcf</t>
+  </si>
+  <si>
+    <t>EIC0016</t>
+  </si>
+  <si>
+    <t>EIC0012</t>
+  </si>
+  <si>
+    <t>jas</t>
+  </si>
+  <si>
+    <t>EIC0023</t>
+  </si>
+  <si>
+    <t>CMMOPS</t>
+  </si>
+  <si>
+    <t>EIC0019</t>
+  </si>
+  <si>
+    <t>aas</t>
+  </si>
+  <si>
+    <t>EIC0110</t>
+  </si>
+  <si>
+    <t>rr</t>
+  </si>
+  <si>
+    <t>EIC0111</t>
+  </si>
+  <si>
+    <t>jpf</t>
+  </si>
+  <si>
+    <t>EIC0027</t>
+  </si>
+  <si>
+    <t>JMPC</t>
+  </si>
+  <si>
+    <t>EIC0029</t>
+  </si>
+  <si>
+    <t>eco</t>
+  </si>
+  <si>
+    <t>EIC0085</t>
+  </si>
+  <si>
+    <t>jcl</t>
+  </si>
+  <si>
+    <t>EIC0031</t>
+  </si>
+  <si>
+    <t>mfst</t>
+  </si>
+  <si>
+    <t>EIC0036</t>
+  </si>
+  <si>
+    <t>pfs</t>
+  </si>
+  <si>
+    <t>EIC0048</t>
+  </si>
+  <si>
+    <t>ama</t>
+  </si>
+  <si>
+    <t>EIC0089</t>
+  </si>
+  <si>
+    <t>jgb</t>
+  </si>
+  <si>
+    <t>EIC0090</t>
+  </si>
+  <si>
+    <t>rpr</t>
+  </si>
+  <si>
+    <t>EIC0053</t>
+  </si>
+  <si>
+    <t>als</t>
+  </si>
+  <si>
+    <t>EIC0037</t>
+  </si>
+  <si>
+    <t>mtd</t>
+  </si>
+  <si>
+    <t>rmv</t>
+  </si>
+  <si>
+    <t>EIC0106</t>
+  </si>
+  <si>
+    <t>EIC0107</t>
+  </si>
+  <si>
+    <t>EIC0061</t>
+  </si>
+  <si>
+    <t>gb</t>
+  </si>
+  <si>
+    <t>EIC0063</t>
+  </si>
+  <si>
+    <t>EIC0064</t>
+  </si>
+  <si>
+    <t>emc</t>
+  </si>
+  <si>
+    <t>EIC0065</t>
+  </si>
+  <si>
+    <t>EIC0092</t>
+  </si>
+  <si>
+    <t>EIC0076</t>
+  </si>
+  <si>
+    <t>rcs</t>
+  </si>
+  <si>
+    <t>mta</t>
+  </si>
+  <si>
+    <t>gtd</t>
+  </si>
+  <si>
+    <t>EIC0077</t>
+  </si>
+  <si>
+    <t>apm</t>
+  </si>
+  <si>
+    <t>EIC0078</t>
+  </si>
+  <si>
+    <t>apr</t>
+  </si>
+  <si>
+    <t>EIC0087</t>
+  </si>
+  <si>
+    <t>mcr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,8 +243,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,34 +573,251 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed lots of bugs
</commit_message>
<xml_diff>
--- a/projeto/calendar_generator_engine/src/test/java/professors.xlsx
+++ b/projeto/calendar_generator_engine/src/test/java/professors.xlsx
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>